<commit_message>
edit on general settings and add new action result to add excel sheet to database
</commit_message>
<xml_diff>
--- a/HR_Sys/wwwroot/files/Book1.xlsx
+++ b/HR_Sys/wwwroot/files/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hady Salah\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533E6A9A-2DA4-4B48-B8C6-3CAE04B925B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE44E92-01A1-40C4-B9BC-16D988DBC624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{174A33C0-DDA3-48E5-961B-7DCCE8371C30}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{174A33C0-DDA3-48E5-961B-7DCCE8371C30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t xml:space="preserve">14/12/2021  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14/12/2021 </t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -381,19 +392,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F838758-876F-4352-ADA2-F9CDA793C387}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="3" width="28.77734375" customWidth="1"/>
+    <col min="3" max="4" width="28.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -403,11 +414,14 @@
       <c r="C1" s="1">
         <v>44542.666666666664</v>
       </c>
-      <c r="D1" t="b">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -417,7 +431,10 @@
       <c r="C2" s="1">
         <v>44542.666666666664</v>
       </c>
-      <c r="D2" t="b">
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Logic of attendance employee
</commit_message>
<xml_diff>
--- a/HR_Sys/wwwroot/files/Book1.xlsx
+++ b/HR_Sys/wwwroot/files/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hady Salah\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE44E92-01A1-40C4-B9BC-16D988DBC624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5802BB1F-BCC3-4F71-A186-28460E2FEADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{174A33C0-DDA3-48E5-961B-7DCCE8371C30}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{174A33C0-DDA3-48E5-961B-7DCCE8371C30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,17 +31,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t xml:space="preserve">14/12/2021  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">14/12/2021 </t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -395,7 +384,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -406,16 +395,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1">
         <v>44542.375</v>
       </c>
       <c r="C1" s="1">
-        <v>44542.666666666664</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>44542.708333333336</v>
+      </c>
+      <c r="D1" s="1">
+        <v>44542</v>
       </c>
       <c r="E1" t="b">
         <v>0</v>
@@ -423,16 +412,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>44542.375</v>
       </c>
       <c r="C2" s="1">
-        <v>44542.666666666664</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>44542.625</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44542</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
handling some logic in excel and new migration
</commit_message>
<xml_diff>
--- a/HR_Sys/wwwroot/files/Book1.xlsx
+++ b/HR_Sys/wwwroot/files/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hady Salah\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5802BB1F-BCC3-4F71-A186-28460E2FEADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464DE028-5A88-4EAA-8BF0-09F4E919B43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{174A33C0-DDA3-48E5-961B-7DCCE8371C30}"/>
   </bookViews>
@@ -384,7 +384,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -397,9 +397,7 @@
       <c r="A1">
         <v>5</v>
       </c>
-      <c r="B1" s="1">
-        <v>44542.375</v>
-      </c>
+      <c r="B1" s="1"/>
       <c r="C1" s="1">
         <v>44542.708333333336</v>
       </c>

</xml_diff>

<commit_message>
edit report paging and searching
</commit_message>
<xml_diff>
--- a/HR_Sys/wwwroot/files/Book1.xlsx
+++ b/HR_Sys/wwwroot/files/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hady Salah\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464DE028-5A88-4EAA-8BF0-09F4E919B43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B32E16A-B574-4F31-BB41-93995FFAC3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{174A33C0-DDA3-48E5-961B-7DCCE8371C30}"/>
   </bookViews>
@@ -383,8 +383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F838758-876F-4352-ADA2-F9CDA793C387}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -397,7 +397,9 @@
       <c r="A1">
         <v>5</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="1">
+        <v>44542.375</v>
+      </c>
       <c r="C1" s="1">
         <v>44542.708333333336</v>
       </c>

</xml_diff>

<commit_message>
logic of adding extra amount and extra hours from excel sheet to database
</commit_message>
<xml_diff>
--- a/HR_Sys/wwwroot/files/Book1.xlsx
+++ b/HR_Sys/wwwroot/files/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hady Salah\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B32E16A-B574-4F31-BB41-93995FFAC3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C887FD4D-C7C0-4DF1-AAB7-013EC0883D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{174A33C0-DDA3-48E5-961B-7DCCE8371C30}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{174A33C0-DDA3-48E5-961B-7DCCE8371C30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F838758-876F-4352-ADA2-F9CDA793C387}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -395,13 +395,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1">
         <v>44542.375</v>
       </c>
       <c r="C1" s="1">
-        <v>44542.708333333336</v>
+        <v>44542.666666666664</v>
       </c>
       <c r="D1" s="1">
         <v>44542</v>
@@ -415,7 +415,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>44542.375</v>
+        <v>44542.333333333336</v>
       </c>
       <c r="C2" s="1">
         <v>44542.625</v>
@@ -424,6 +424,125 @@
         <v>44542</v>
       </c>
       <c r="E2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44542.333333333336</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44542.625</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44542</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44542.333333333336</v>
+      </c>
+      <c r="C4" s="1">
+        <v>44542.625</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44542</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44542.333333333336</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44542.625</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44542</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44542.333333333336</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44542.625</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44542</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44542.333333333336</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44542.625</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44542</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44542.333333333336</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44542.625</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44542</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44542.333333333336</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44542.625</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44542</v>
+      </c>
+      <c r="E9" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>